<commit_message>
ConditionBit를 이용한 퀘스트 수주 (GAME_START만)
</commit_message>
<xml_diff>
--- a/Assets/ExcelDatas/QuestLocalizationTable.xlsx
+++ b/Assets/ExcelDatas/QuestLocalizationTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Project-H9\Assets\ExcelDatas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE22F8B-D6F8-4EEF-AD71-0BC0EB3F5BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8464249B-FC65-44A8-AD0C-0FAFDA539129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18585" yWindow="255" windowWidth="16950" windowHeight="15465" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8025" yWindow="165" windowWidth="20640" windowHeight="15465" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>index</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -39,10 +39,6 @@
   </si>
   <si>
     <t>NULL Data</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>주석</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -420,10 +416,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -433,7 +429,7 @@
     <col min="3" max="3" width="21.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -443,11 +439,8 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -458,70 +451,70 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>